<commit_message>
19.11.18 báo cáo ngày
</commit_message>
<xml_diff>
--- a/DailyReport/DailyReport_DuongLT.xlsx
+++ b/DailyReport/DailyReport_DuongLT.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="34">
   <si>
     <t xml:space="preserve">No.</t>
   </si>
@@ -93,6 +93,18 @@
   </si>
   <si>
     <t xml:space="preserve">Thiết kế lại side hiên thị danh sách </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thiết kế giao diện reponsive live chat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ẩn danh sách conversation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chức năng ẩn hiện form lưu thông tin khách hàng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tạo chức năng ẩn hiện danh sách conversation</t>
   </si>
   <si>
     <t xml:space="preserve">!</t>
@@ -556,9 +568,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>96</xdr:col>
-      <xdr:colOff>50040</xdr:colOff>
+      <xdr:colOff>49680</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>135000</xdr:rowOff>
+      <xdr:rowOff>134640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -568,7 +580,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="16608960" y="474480"/>
-          <a:ext cx="2745000" cy="1946520"/>
+          <a:ext cx="2744640" cy="1946160"/>
         </a:xfrm>
         <a:prstGeom prst="foldedCorner">
           <a:avLst>
@@ -662,9 +674,9 @@
   <dimension ref="A1:CA72"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="AS18" activeCellId="0" sqref="AS18"/>
+      <selection pane="bottomLeft" activeCell="AS26" activeCellId="0" sqref="AS26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2397,7 +2409,7 @@
       <c r="AN20" s="20"/>
       <c r="AO20" s="20"/>
       <c r="AP20" s="21" t="n">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="AQ20" s="21"/>
       <c r="AR20" s="21"/>
@@ -2528,39 +2540,41 @@
       </c>
       <c r="B22" s="16"/>
       <c r="C22" s="17"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="20"/>
-      <c r="K22" s="20"/>
-      <c r="L22" s="20"/>
-      <c r="M22" s="20"/>
-      <c r="N22" s="20"/>
-      <c r="O22" s="20"/>
-      <c r="P22" s="20"/>
-      <c r="Q22" s="20"/>
-      <c r="R22" s="20"/>
-      <c r="S22" s="20"/>
-      <c r="T22" s="20"/>
-      <c r="U22" s="20"/>
-      <c r="V22" s="20"/>
-      <c r="W22" s="20"/>
-      <c r="X22" s="20"/>
-      <c r="Y22" s="20"/>
-      <c r="Z22" s="20"/>
-      <c r="AA22" s="20"/>
-      <c r="AB22" s="20"/>
-      <c r="AC22" s="20"/>
-      <c r="AD22" s="20"/>
-      <c r="AE22" s="20"/>
-      <c r="AF22" s="18"/>
-      <c r="AG22" s="18"/>
-      <c r="AH22" s="18"/>
-      <c r="AI22" s="18"/>
-      <c r="AJ22" s="18"/>
+      <c r="D22" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="26"/>
+      <c r="J22" s="26"/>
+      <c r="K22" s="26"/>
+      <c r="L22" s="26"/>
+      <c r="M22" s="26"/>
+      <c r="N22" s="26"/>
+      <c r="O22" s="26"/>
+      <c r="P22" s="26"/>
+      <c r="Q22" s="26"/>
+      <c r="R22" s="26"/>
+      <c r="S22" s="26"/>
+      <c r="T22" s="26"/>
+      <c r="U22" s="26"/>
+      <c r="V22" s="26"/>
+      <c r="W22" s="26"/>
+      <c r="X22" s="26"/>
+      <c r="Y22" s="26"/>
+      <c r="Z22" s="26"/>
+      <c r="AA22" s="26"/>
+      <c r="AB22" s="26"/>
+      <c r="AC22" s="26"/>
+      <c r="AD22" s="26"/>
+      <c r="AE22" s="26"/>
+      <c r="AF22" s="11"/>
+      <c r="AG22" s="11"/>
+      <c r="AH22" s="11"/>
+      <c r="AI22" s="11"/>
+      <c r="AJ22" s="11"/>
       <c r="AK22" s="20"/>
       <c r="AL22" s="20"/>
       <c r="AM22" s="20"/>
@@ -2611,7 +2625,9 @@
       </c>
       <c r="B23" s="16"/>
       <c r="C23" s="17"/>
-      <c r="D23" s="20"/>
+      <c r="D23" s="20" t="s">
+        <v>25</v>
+      </c>
       <c r="E23" s="20"/>
       <c r="F23" s="20"/>
       <c r="G23" s="20"/>
@@ -2639,7 +2655,9 @@
       <c r="AC23" s="20"/>
       <c r="AD23" s="20"/>
       <c r="AE23" s="20"/>
-      <c r="AF23" s="18"/>
+      <c r="AF23" s="18" t="n">
+        <v>43421</v>
+      </c>
       <c r="AG23" s="18"/>
       <c r="AH23" s="18"/>
       <c r="AI23" s="18"/>
@@ -2649,10 +2667,14 @@
       <c r="AM23" s="20"/>
       <c r="AN23" s="20"/>
       <c r="AO23" s="20"/>
-      <c r="AP23" s="21"/>
+      <c r="AP23" s="21" t="n">
+        <v>1</v>
+      </c>
       <c r="AQ23" s="21"/>
       <c r="AR23" s="21"/>
-      <c r="AS23" s="20"/>
+      <c r="AS23" s="20" t="s">
+        <v>10</v>
+      </c>
       <c r="AT23" s="20"/>
       <c r="AU23" s="20"/>
       <c r="AV23" s="20"/>
@@ -2694,7 +2716,9 @@
       </c>
       <c r="B24" s="16"/>
       <c r="C24" s="17"/>
-      <c r="D24" s="20"/>
+      <c r="D24" s="20" t="s">
+        <v>26</v>
+      </c>
       <c r="E24" s="20"/>
       <c r="F24" s="20"/>
       <c r="G24" s="20"/>
@@ -2722,7 +2746,9 @@
       <c r="AC24" s="20"/>
       <c r="AD24" s="20"/>
       <c r="AE24" s="20"/>
-      <c r="AF24" s="18"/>
+      <c r="AF24" s="18" t="n">
+        <v>43421</v>
+      </c>
       <c r="AG24" s="18"/>
       <c r="AH24" s="18"/>
       <c r="AI24" s="18"/>
@@ -2732,10 +2758,14 @@
       <c r="AM24" s="20"/>
       <c r="AN24" s="20"/>
       <c r="AO24" s="20"/>
-      <c r="AP24" s="21"/>
+      <c r="AP24" s="21" t="n">
+        <v>1</v>
+      </c>
       <c r="AQ24" s="21"/>
       <c r="AR24" s="21"/>
-      <c r="AS24" s="20"/>
+      <c r="AS24" s="20" t="s">
+        <v>10</v>
+      </c>
       <c r="AT24" s="20"/>
       <c r="AU24" s="20"/>
       <c r="AV24" s="20"/>
@@ -2860,7 +2890,9 @@
       </c>
       <c r="B26" s="16"/>
       <c r="C26" s="17"/>
-      <c r="D26" s="20"/>
+      <c r="D26" s="20" t="s">
+        <v>27</v>
+      </c>
       <c r="E26" s="20"/>
       <c r="F26" s="20"/>
       <c r="G26" s="20"/>
@@ -2888,7 +2920,9 @@
       <c r="AC26" s="20"/>
       <c r="AD26" s="20"/>
       <c r="AE26" s="20"/>
-      <c r="AF26" s="18"/>
+      <c r="AF26" s="18" t="n">
+        <v>43423</v>
+      </c>
       <c r="AG26" s="18"/>
       <c r="AH26" s="18"/>
       <c r="AI26" s="18"/>
@@ -2898,10 +2932,14 @@
       <c r="AM26" s="20"/>
       <c r="AN26" s="20"/>
       <c r="AO26" s="20"/>
-      <c r="AP26" s="21"/>
+      <c r="AP26" s="21" t="n">
+        <v>0.9</v>
+      </c>
       <c r="AQ26" s="21"/>
       <c r="AR26" s="21"/>
-      <c r="AS26" s="20"/>
+      <c r="AS26" s="20" t="s">
+        <v>10</v>
+      </c>
       <c r="AT26" s="20"/>
       <c r="AU26" s="20"/>
       <c r="AV26" s="20"/>
@@ -4271,7 +4309,7 @@
       </c>
       <c r="B43" s="16"/>
       <c r="C43" s="17" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D43" s="20"/>
       <c r="E43" s="20"/>
@@ -7310,7 +7348,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>10</v>
@@ -7318,17 +7356,17 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7338,7 +7376,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
20.11.18 báo cáo ngày
</commit_message>
<xml_diff>
--- a/DailyReport/DailyReport_DuongLT.xlsx
+++ b/DailyReport/DailyReport_DuongLT.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="35">
   <si>
     <t xml:space="preserve">No.</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t xml:space="preserve">Tạo chức năng ẩn hiện danh sách conversation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hoàn thiện giao diện live chat (chứa test lỗi)</t>
   </si>
   <si>
     <t xml:space="preserve">!</t>
@@ -568,9 +571,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>96</xdr:col>
-      <xdr:colOff>49680</xdr:colOff>
+      <xdr:colOff>49320</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>134640</xdr:rowOff>
+      <xdr:rowOff>134280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -580,7 +583,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="16608960" y="474480"/>
-          <a:ext cx="2744640" cy="1946160"/>
+          <a:ext cx="2744280" cy="1945800"/>
         </a:xfrm>
         <a:prstGeom prst="foldedCorner">
           <a:avLst>
@@ -676,7 +679,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="AS26" activeCellId="0" sqref="AS26"/>
+      <selection pane="bottomLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3064,7 +3067,9 @@
       </c>
       <c r="B28" s="16"/>
       <c r="C28" s="17"/>
-      <c r="D28" s="20"/>
+      <c r="D28" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="E28" s="20"/>
       <c r="F28" s="20"/>
       <c r="G28" s="20"/>
@@ -3092,7 +3097,9 @@
       <c r="AC28" s="20"/>
       <c r="AD28" s="20"/>
       <c r="AE28" s="20"/>
-      <c r="AF28" s="18"/>
+      <c r="AF28" s="18" t="n">
+        <v>43424</v>
+      </c>
       <c r="AG28" s="18"/>
       <c r="AH28" s="18"/>
       <c r="AI28" s="18"/>
@@ -3102,10 +3109,14 @@
       <c r="AM28" s="20"/>
       <c r="AN28" s="20"/>
       <c r="AO28" s="20"/>
-      <c r="AP28" s="21"/>
+      <c r="AP28" s="21" t="n">
+        <v>1</v>
+      </c>
       <c r="AQ28" s="21"/>
       <c r="AR28" s="21"/>
-      <c r="AS28" s="20"/>
+      <c r="AS28" s="20" t="s">
+        <v>10</v>
+      </c>
       <c r="AT28" s="20"/>
       <c r="AU28" s="20"/>
       <c r="AV28" s="20"/>
@@ -4309,7 +4320,7 @@
       </c>
       <c r="B43" s="16"/>
       <c r="C43" s="17" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D43" s="20"/>
       <c r="E43" s="20"/>
@@ -7348,7 +7359,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>10</v>
@@ -7356,17 +7367,17 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7376,7 +7387,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
26.11.18 báo cáo ngày
</commit_message>
<xml_diff>
--- a/DailyReport/DailyReport_DuongLT.xlsx
+++ b/DailyReport/DailyReport_DuongLT.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="44">
   <si>
     <t xml:space="preserve">No.</t>
   </si>
@@ -131,7 +131,13 @@
     <t xml:space="preserve">ẩn chatbox để chỉ luôn hiển thị tối đa 3 chatbox</t>
   </si>
   <si>
-    <t xml:space="preserve">!</t>
+    <t xml:space="preserve">ẩn chatbox để chỉ luôn hiển thị tối đa 3 chatbox &lt;Tiếp&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sửa lỗi load sai danh sách chatbox ẩn sau khi đóng một chatbox bất kì</t>
+  </si>
+  <si>
+    <t xml:space="preserve">click nút “chat” trên thông báo có khác truy cập thì chatbox mới phải hiển lên đầu</t>
   </si>
   <si>
     <t xml:space="preserve">AnhND</t>
@@ -158,7 +164,7 @@
     <numFmt numFmtId="165" formatCode="YYYY/MM/DD"/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -196,6 +202,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -362,7 +374,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -511,6 +523,10 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -606,9 +622,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>96</xdr:col>
-      <xdr:colOff>48960</xdr:colOff>
+      <xdr:colOff>48600</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>133920</xdr:rowOff>
+      <xdr:rowOff>133560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -618,7 +634,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="16948800" y="497520"/>
-          <a:ext cx="2810520" cy="2112840"/>
+          <a:ext cx="2810160" cy="2112480"/>
         </a:xfrm>
         <a:prstGeom prst="foldedCorner">
           <a:avLst>
@@ -714,7 +730,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="BG38" activeCellId="0" sqref="BG38"/>
+      <selection pane="bottomLeft" activeCell="BG44" activeCellId="0" sqref="BG44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4156,7 +4172,9 @@
       </c>
       <c r="B40" s="16"/>
       <c r="C40" s="17"/>
-      <c r="D40" s="20"/>
+      <c r="D40" s="20" t="s">
+        <v>36</v>
+      </c>
       <c r="E40" s="20"/>
       <c r="F40" s="20"/>
       <c r="G40" s="20"/>
@@ -4184,7 +4202,9 @@
       <c r="AC40" s="20"/>
       <c r="AD40" s="20"/>
       <c r="AE40" s="20"/>
-      <c r="AF40" s="18"/>
+      <c r="AF40" s="18" t="n">
+        <v>43428</v>
+      </c>
       <c r="AG40" s="18"/>
       <c r="AH40" s="18"/>
       <c r="AI40" s="18"/>
@@ -4194,10 +4214,14 @@
       <c r="AM40" s="20"/>
       <c r="AN40" s="20"/>
       <c r="AO40" s="20"/>
-      <c r="AP40" s="21"/>
+      <c r="AP40" s="21" t="n">
+        <v>0.8</v>
+      </c>
       <c r="AQ40" s="21"/>
       <c r="AR40" s="21"/>
-      <c r="AS40" s="20"/>
+      <c r="AS40" s="20" t="s">
+        <v>10</v>
+      </c>
       <c r="AT40" s="20"/>
       <c r="AU40" s="20"/>
       <c r="AV40" s="20"/>
@@ -4316,41 +4340,45 @@
       <c r="BZ41" s="19"/>
       <c r="CA41" s="19"/>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="16" t="n">
         <v>40</v>
       </c>
       <c r="B42" s="16"/>
       <c r="C42" s="17"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="20"/>
-      <c r="G42" s="20"/>
-      <c r="H42" s="20"/>
-      <c r="I42" s="20"/>
-      <c r="J42" s="20"/>
-      <c r="K42" s="20"/>
-      <c r="L42" s="20"/>
-      <c r="M42" s="20"/>
-      <c r="N42" s="20"/>
-      <c r="O42" s="20"/>
-      <c r="P42" s="20"/>
-      <c r="Q42" s="20"/>
-      <c r="R42" s="20"/>
-      <c r="S42" s="20"/>
-      <c r="T42" s="20"/>
-      <c r="U42" s="20"/>
-      <c r="V42" s="20"/>
-      <c r="W42" s="20"/>
-      <c r="X42" s="20"/>
-      <c r="Y42" s="20"/>
-      <c r="Z42" s="20"/>
-      <c r="AA42" s="20"/>
-      <c r="AB42" s="20"/>
-      <c r="AC42" s="20"/>
-      <c r="AD42" s="20"/>
-      <c r="AE42" s="20"/>
-      <c r="AF42" s="18"/>
+      <c r="D42" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="E42" s="37"/>
+      <c r="F42" s="37"/>
+      <c r="G42" s="37"/>
+      <c r="H42" s="37"/>
+      <c r="I42" s="37"/>
+      <c r="J42" s="37"/>
+      <c r="K42" s="37"/>
+      <c r="L42" s="37"/>
+      <c r="M42" s="37"/>
+      <c r="N42" s="37"/>
+      <c r="O42" s="37"/>
+      <c r="P42" s="37"/>
+      <c r="Q42" s="37"/>
+      <c r="R42" s="37"/>
+      <c r="S42" s="37"/>
+      <c r="T42" s="37"/>
+      <c r="U42" s="37"/>
+      <c r="V42" s="37"/>
+      <c r="W42" s="37"/>
+      <c r="X42" s="37"/>
+      <c r="Y42" s="37"/>
+      <c r="Z42" s="37"/>
+      <c r="AA42" s="37"/>
+      <c r="AB42" s="37"/>
+      <c r="AC42" s="37"/>
+      <c r="AD42" s="37"/>
+      <c r="AE42" s="37"/>
+      <c r="AF42" s="18" t="n">
+        <v>43430</v>
+      </c>
       <c r="AG42" s="18"/>
       <c r="AH42" s="18"/>
       <c r="AI42" s="18"/>
@@ -4360,10 +4388,14 @@
       <c r="AM42" s="20"/>
       <c r="AN42" s="20"/>
       <c r="AO42" s="20"/>
-      <c r="AP42" s="21"/>
+      <c r="AP42" s="21" t="n">
+        <v>1</v>
+      </c>
       <c r="AQ42" s="21"/>
       <c r="AR42" s="21"/>
-      <c r="AS42" s="20"/>
+      <c r="AS42" s="20" t="s">
+        <v>10</v>
+      </c>
       <c r="AT42" s="20"/>
       <c r="AU42" s="20"/>
       <c r="AV42" s="20"/>
@@ -4399,15 +4431,15 @@
       <c r="BZ42" s="19"/>
       <c r="CA42" s="19"/>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="16" t="n">
         <v>41</v>
       </c>
       <c r="B43" s="16"/>
-      <c r="C43" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D43" s="20"/>
+      <c r="C43" s="17"/>
+      <c r="D43" s="20" t="s">
+        <v>37</v>
+      </c>
       <c r="E43" s="20"/>
       <c r="F43" s="20"/>
       <c r="G43" s="20"/>
@@ -4435,7 +4467,9 @@
       <c r="AC43" s="20"/>
       <c r="AD43" s="20"/>
       <c r="AE43" s="20"/>
-      <c r="AF43" s="18"/>
+      <c r="AF43" s="18" t="n">
+        <v>43430</v>
+      </c>
       <c r="AG43" s="18"/>
       <c r="AH43" s="18"/>
       <c r="AI43" s="18"/>
@@ -4445,10 +4479,14 @@
       <c r="AM43" s="20"/>
       <c r="AN43" s="20"/>
       <c r="AO43" s="20"/>
-      <c r="AP43" s="21"/>
+      <c r="AP43" s="21" t="n">
+        <v>0.3</v>
+      </c>
       <c r="AQ43" s="21"/>
       <c r="AR43" s="21"/>
-      <c r="AS43" s="20"/>
+      <c r="AS43" s="20" t="s">
+        <v>10</v>
+      </c>
       <c r="AT43" s="20"/>
       <c r="AU43" s="20"/>
       <c r="AV43" s="20"/>
@@ -4490,7 +4528,9 @@
       </c>
       <c r="B44" s="16"/>
       <c r="C44" s="17"/>
-      <c r="D44" s="20"/>
+      <c r="D44" s="20" t="s">
+        <v>38</v>
+      </c>
       <c r="E44" s="20"/>
       <c r="F44" s="20"/>
       <c r="G44" s="20"/>
@@ -4518,7 +4558,9 @@
       <c r="AC44" s="20"/>
       <c r="AD44" s="20"/>
       <c r="AE44" s="20"/>
-      <c r="AF44" s="18"/>
+      <c r="AF44" s="18" t="n">
+        <v>43430</v>
+      </c>
       <c r="AG44" s="18"/>
       <c r="AH44" s="18"/>
       <c r="AI44" s="18"/>
@@ -4528,10 +4570,14 @@
       <c r="AM44" s="20"/>
       <c r="AN44" s="20"/>
       <c r="AO44" s="20"/>
-      <c r="AP44" s="21"/>
+      <c r="AP44" s="21" t="n">
+        <v>0.1</v>
+      </c>
       <c r="AQ44" s="21"/>
       <c r="AR44" s="21"/>
-      <c r="AS44" s="20"/>
+      <c r="AS44" s="20" t="s">
+        <v>10</v>
+      </c>
       <c r="AT44" s="20"/>
       <c r="AU44" s="20"/>
       <c r="AV44" s="20"/>
@@ -5942,20 +5988,20 @@
       <c r="AP61" s="21"/>
       <c r="AQ61" s="21"/>
       <c r="AR61" s="21"/>
-      <c r="AS61" s="37"/>
-      <c r="AT61" s="37"/>
-      <c r="AU61" s="37"/>
-      <c r="AV61" s="37"/>
-      <c r="AW61" s="37"/>
-      <c r="AX61" s="37"/>
-      <c r="AY61" s="37"/>
-      <c r="AZ61" s="37"/>
-      <c r="BA61" s="37"/>
-      <c r="BB61" s="37"/>
-      <c r="BC61" s="37"/>
-      <c r="BD61" s="37"/>
-      <c r="BE61" s="37"/>
-      <c r="BF61" s="37"/>
+      <c r="AS61" s="38"/>
+      <c r="AT61" s="38"/>
+      <c r="AU61" s="38"/>
+      <c r="AV61" s="38"/>
+      <c r="AW61" s="38"/>
+      <c r="AX61" s="38"/>
+      <c r="AY61" s="38"/>
+      <c r="AZ61" s="38"/>
+      <c r="BA61" s="38"/>
+      <c r="BB61" s="38"/>
+      <c r="BC61" s="38"/>
+      <c r="BD61" s="38"/>
+      <c r="BE61" s="38"/>
+      <c r="BF61" s="38"/>
       <c r="BG61" s="16"/>
       <c r="BH61" s="16"/>
       <c r="BI61" s="16"/>
@@ -6025,41 +6071,41 @@
       <c r="AP62" s="21"/>
       <c r="AQ62" s="21"/>
       <c r="AR62" s="21"/>
-      <c r="AS62" s="37"/>
-      <c r="AT62" s="37"/>
-      <c r="AU62" s="37"/>
-      <c r="AV62" s="37"/>
-      <c r="AW62" s="37"/>
-      <c r="AX62" s="37"/>
-      <c r="AY62" s="37"/>
-      <c r="AZ62" s="37"/>
-      <c r="BA62" s="37"/>
-      <c r="BB62" s="37"/>
-      <c r="BC62" s="37"/>
-      <c r="BD62" s="37"/>
-      <c r="BE62" s="37"/>
-      <c r="BF62" s="37"/>
-      <c r="BG62" s="38"/>
-      <c r="BH62" s="38"/>
-      <c r="BI62" s="38"/>
-      <c r="BJ62" s="38"/>
-      <c r="BK62" s="38"/>
-      <c r="BL62" s="38"/>
-      <c r="BM62" s="38"/>
-      <c r="BN62" s="38"/>
-      <c r="BO62" s="38"/>
-      <c r="BP62" s="38"/>
-      <c r="BQ62" s="38"/>
-      <c r="BR62" s="38"/>
-      <c r="BS62" s="38"/>
-      <c r="BT62" s="38"/>
-      <c r="BU62" s="38"/>
-      <c r="BV62" s="38"/>
-      <c r="BW62" s="38"/>
-      <c r="BX62" s="38"/>
-      <c r="BY62" s="38"/>
-      <c r="BZ62" s="38"/>
-      <c r="CA62" s="38"/>
+      <c r="AS62" s="38"/>
+      <c r="AT62" s="38"/>
+      <c r="AU62" s="38"/>
+      <c r="AV62" s="38"/>
+      <c r="AW62" s="38"/>
+      <c r="AX62" s="38"/>
+      <c r="AY62" s="38"/>
+      <c r="AZ62" s="38"/>
+      <c r="BA62" s="38"/>
+      <c r="BB62" s="38"/>
+      <c r="BC62" s="38"/>
+      <c r="BD62" s="38"/>
+      <c r="BE62" s="38"/>
+      <c r="BF62" s="38"/>
+      <c r="BG62" s="39"/>
+      <c r="BH62" s="39"/>
+      <c r="BI62" s="39"/>
+      <c r="BJ62" s="39"/>
+      <c r="BK62" s="39"/>
+      <c r="BL62" s="39"/>
+      <c r="BM62" s="39"/>
+      <c r="BN62" s="39"/>
+      <c r="BO62" s="39"/>
+      <c r="BP62" s="39"/>
+      <c r="BQ62" s="39"/>
+      <c r="BR62" s="39"/>
+      <c r="BS62" s="39"/>
+      <c r="BT62" s="39"/>
+      <c r="BU62" s="39"/>
+      <c r="BV62" s="39"/>
+      <c r="BW62" s="39"/>
+      <c r="BX62" s="39"/>
+      <c r="BY62" s="39"/>
+      <c r="BZ62" s="39"/>
+      <c r="CA62" s="39"/>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="16" t="n">
@@ -6108,20 +6154,20 @@
       <c r="AP63" s="21"/>
       <c r="AQ63" s="21"/>
       <c r="AR63" s="21"/>
-      <c r="AS63" s="37"/>
-      <c r="AT63" s="37"/>
-      <c r="AU63" s="37"/>
-      <c r="AV63" s="37"/>
-      <c r="AW63" s="37"/>
-      <c r="AX63" s="37"/>
-      <c r="AY63" s="37"/>
-      <c r="AZ63" s="37"/>
-      <c r="BA63" s="37"/>
-      <c r="BB63" s="37"/>
-      <c r="BC63" s="37"/>
-      <c r="BD63" s="37"/>
-      <c r="BE63" s="37"/>
-      <c r="BF63" s="37"/>
+      <c r="AS63" s="38"/>
+      <c r="AT63" s="38"/>
+      <c r="AU63" s="38"/>
+      <c r="AV63" s="38"/>
+      <c r="AW63" s="38"/>
+      <c r="AX63" s="38"/>
+      <c r="AY63" s="38"/>
+      <c r="AZ63" s="38"/>
+      <c r="BA63" s="38"/>
+      <c r="BB63" s="38"/>
+      <c r="BC63" s="38"/>
+      <c r="BD63" s="38"/>
+      <c r="BE63" s="38"/>
+      <c r="BF63" s="38"/>
       <c r="BG63" s="16"/>
       <c r="BH63" s="16"/>
       <c r="BI63" s="16"/>
@@ -6178,11 +6224,11 @@
       <c r="AC64" s="12"/>
       <c r="AD64" s="12"/>
       <c r="AE64" s="12"/>
-      <c r="AF64" s="39"/>
-      <c r="AG64" s="39"/>
-      <c r="AH64" s="39"/>
-      <c r="AI64" s="39"/>
-      <c r="AJ64" s="39"/>
+      <c r="AF64" s="40"/>
+      <c r="AG64" s="40"/>
+      <c r="AH64" s="40"/>
+      <c r="AI64" s="40"/>
+      <c r="AJ64" s="40"/>
       <c r="AK64" s="12"/>
       <c r="AL64" s="12"/>
       <c r="AM64" s="12"/>
@@ -6191,41 +6237,41 @@
       <c r="AP64" s="13"/>
       <c r="AQ64" s="13"/>
       <c r="AR64" s="13"/>
-      <c r="AS64" s="37"/>
-      <c r="AT64" s="37"/>
-      <c r="AU64" s="37"/>
-      <c r="AV64" s="37"/>
-      <c r="AW64" s="37"/>
-      <c r="AX64" s="37"/>
-      <c r="AY64" s="37"/>
-      <c r="AZ64" s="37"/>
-      <c r="BA64" s="37"/>
-      <c r="BB64" s="37"/>
-      <c r="BC64" s="37"/>
-      <c r="BD64" s="37"/>
-      <c r="BE64" s="37"/>
-      <c r="BF64" s="37"/>
-      <c r="BG64" s="38"/>
-      <c r="BH64" s="38"/>
-      <c r="BI64" s="38"/>
-      <c r="BJ64" s="38"/>
-      <c r="BK64" s="38"/>
-      <c r="BL64" s="38"/>
-      <c r="BM64" s="38"/>
-      <c r="BN64" s="38"/>
-      <c r="BO64" s="38"/>
-      <c r="BP64" s="38"/>
-      <c r="BQ64" s="38"/>
-      <c r="BR64" s="38"/>
-      <c r="BS64" s="38"/>
-      <c r="BT64" s="38"/>
-      <c r="BU64" s="38"/>
-      <c r="BV64" s="38"/>
-      <c r="BW64" s="38"/>
-      <c r="BX64" s="38"/>
-      <c r="BY64" s="38"/>
-      <c r="BZ64" s="38"/>
-      <c r="CA64" s="38"/>
+      <c r="AS64" s="38"/>
+      <c r="AT64" s="38"/>
+      <c r="AU64" s="38"/>
+      <c r="AV64" s="38"/>
+      <c r="AW64" s="38"/>
+      <c r="AX64" s="38"/>
+      <c r="AY64" s="38"/>
+      <c r="AZ64" s="38"/>
+      <c r="BA64" s="38"/>
+      <c r="BB64" s="38"/>
+      <c r="BC64" s="38"/>
+      <c r="BD64" s="38"/>
+      <c r="BE64" s="38"/>
+      <c r="BF64" s="38"/>
+      <c r="BG64" s="39"/>
+      <c r="BH64" s="39"/>
+      <c r="BI64" s="39"/>
+      <c r="BJ64" s="39"/>
+      <c r="BK64" s="39"/>
+      <c r="BL64" s="39"/>
+      <c r="BM64" s="39"/>
+      <c r="BN64" s="39"/>
+      <c r="BO64" s="39"/>
+      <c r="BP64" s="39"/>
+      <c r="BQ64" s="39"/>
+      <c r="BR64" s="39"/>
+      <c r="BS64" s="39"/>
+      <c r="BT64" s="39"/>
+      <c r="BU64" s="39"/>
+      <c r="BV64" s="39"/>
+      <c r="BW64" s="39"/>
+      <c r="BX64" s="39"/>
+      <c r="BY64" s="39"/>
+      <c r="BZ64" s="39"/>
+      <c r="CA64" s="39"/>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="16" t="n">
@@ -6274,20 +6320,20 @@
       <c r="AP65" s="21"/>
       <c r="AQ65" s="21"/>
       <c r="AR65" s="21"/>
-      <c r="AS65" s="37"/>
-      <c r="AT65" s="37"/>
-      <c r="AU65" s="37"/>
-      <c r="AV65" s="37"/>
-      <c r="AW65" s="37"/>
-      <c r="AX65" s="37"/>
-      <c r="AY65" s="37"/>
-      <c r="AZ65" s="37"/>
-      <c r="BA65" s="37"/>
-      <c r="BB65" s="37"/>
-      <c r="BC65" s="37"/>
-      <c r="BD65" s="37"/>
-      <c r="BE65" s="37"/>
-      <c r="BF65" s="37"/>
+      <c r="AS65" s="38"/>
+      <c r="AT65" s="38"/>
+      <c r="AU65" s="38"/>
+      <c r="AV65" s="38"/>
+      <c r="AW65" s="38"/>
+      <c r="AX65" s="38"/>
+      <c r="AY65" s="38"/>
+      <c r="AZ65" s="38"/>
+      <c r="BA65" s="38"/>
+      <c r="BB65" s="38"/>
+      <c r="BC65" s="38"/>
+      <c r="BD65" s="38"/>
+      <c r="BE65" s="38"/>
+      <c r="BF65" s="38"/>
       <c r="BG65" s="16"/>
       <c r="BH65" s="16"/>
       <c r="BI65" s="16"/>
@@ -6357,20 +6403,20 @@
       <c r="AP66" s="13"/>
       <c r="AQ66" s="13"/>
       <c r="AR66" s="13"/>
-      <c r="AS66" s="37"/>
-      <c r="AT66" s="37"/>
-      <c r="AU66" s="37"/>
-      <c r="AV66" s="37"/>
-      <c r="AW66" s="37"/>
-      <c r="AX66" s="37"/>
-      <c r="AY66" s="37"/>
-      <c r="AZ66" s="37"/>
-      <c r="BA66" s="37"/>
-      <c r="BB66" s="37"/>
-      <c r="BC66" s="37"/>
-      <c r="BD66" s="37"/>
-      <c r="BE66" s="37"/>
-      <c r="BF66" s="37"/>
+      <c r="AS66" s="38"/>
+      <c r="AT66" s="38"/>
+      <c r="AU66" s="38"/>
+      <c r="AV66" s="38"/>
+      <c r="AW66" s="38"/>
+      <c r="AX66" s="38"/>
+      <c r="AY66" s="38"/>
+      <c r="AZ66" s="38"/>
+      <c r="BA66" s="38"/>
+      <c r="BB66" s="38"/>
+      <c r="BC66" s="38"/>
+      <c r="BD66" s="38"/>
+      <c r="BE66" s="38"/>
+      <c r="BF66" s="38"/>
       <c r="BG66" s="16"/>
       <c r="BH66" s="16"/>
       <c r="BI66" s="16"/>
@@ -6440,20 +6486,20 @@
       <c r="AP67" s="13"/>
       <c r="AQ67" s="13"/>
       <c r="AR67" s="13"/>
-      <c r="AS67" s="37"/>
-      <c r="AT67" s="37"/>
-      <c r="AU67" s="37"/>
-      <c r="AV67" s="37"/>
-      <c r="AW67" s="37"/>
-      <c r="AX67" s="37"/>
-      <c r="AY67" s="37"/>
-      <c r="AZ67" s="37"/>
-      <c r="BA67" s="37"/>
-      <c r="BB67" s="37"/>
-      <c r="BC67" s="37"/>
-      <c r="BD67" s="37"/>
-      <c r="BE67" s="37"/>
-      <c r="BF67" s="37"/>
+      <c r="AS67" s="38"/>
+      <c r="AT67" s="38"/>
+      <c r="AU67" s="38"/>
+      <c r="AV67" s="38"/>
+      <c r="AW67" s="38"/>
+      <c r="AX67" s="38"/>
+      <c r="AY67" s="38"/>
+      <c r="AZ67" s="38"/>
+      <c r="BA67" s="38"/>
+      <c r="BB67" s="38"/>
+      <c r="BC67" s="38"/>
+      <c r="BD67" s="38"/>
+      <c r="BE67" s="38"/>
+      <c r="BF67" s="38"/>
       <c r="BG67" s="16"/>
       <c r="BH67" s="16"/>
       <c r="BI67" s="16"/>
@@ -6523,20 +6569,20 @@
       <c r="AP68" s="13"/>
       <c r="AQ68" s="13"/>
       <c r="AR68" s="13"/>
-      <c r="AS68" s="37"/>
-      <c r="AT68" s="37"/>
-      <c r="AU68" s="37"/>
-      <c r="AV68" s="37"/>
-      <c r="AW68" s="37"/>
-      <c r="AX68" s="37"/>
-      <c r="AY68" s="37"/>
-      <c r="AZ68" s="37"/>
-      <c r="BA68" s="37"/>
-      <c r="BB68" s="37"/>
-      <c r="BC68" s="37"/>
-      <c r="BD68" s="37"/>
-      <c r="BE68" s="37"/>
-      <c r="BF68" s="37"/>
+      <c r="AS68" s="38"/>
+      <c r="AT68" s="38"/>
+      <c r="AU68" s="38"/>
+      <c r="AV68" s="38"/>
+      <c r="AW68" s="38"/>
+      <c r="AX68" s="38"/>
+      <c r="AY68" s="38"/>
+      <c r="AZ68" s="38"/>
+      <c r="BA68" s="38"/>
+      <c r="BB68" s="38"/>
+      <c r="BC68" s="38"/>
+      <c r="BD68" s="38"/>
+      <c r="BE68" s="38"/>
+      <c r="BF68" s="38"/>
       <c r="BG68" s="16"/>
       <c r="BH68" s="16"/>
       <c r="BI68" s="16"/>
@@ -6606,20 +6652,20 @@
       <c r="AP69" s="13"/>
       <c r="AQ69" s="13"/>
       <c r="AR69" s="13"/>
-      <c r="AS69" s="37"/>
-      <c r="AT69" s="37"/>
-      <c r="AU69" s="37"/>
-      <c r="AV69" s="37"/>
-      <c r="AW69" s="37"/>
-      <c r="AX69" s="37"/>
-      <c r="AY69" s="37"/>
-      <c r="AZ69" s="37"/>
-      <c r="BA69" s="37"/>
-      <c r="BB69" s="37"/>
-      <c r="BC69" s="37"/>
-      <c r="BD69" s="37"/>
-      <c r="BE69" s="37"/>
-      <c r="BF69" s="37"/>
+      <c r="AS69" s="38"/>
+      <c r="AT69" s="38"/>
+      <c r="AU69" s="38"/>
+      <c r="AV69" s="38"/>
+      <c r="AW69" s="38"/>
+      <c r="AX69" s="38"/>
+      <c r="AY69" s="38"/>
+      <c r="AZ69" s="38"/>
+      <c r="BA69" s="38"/>
+      <c r="BB69" s="38"/>
+      <c r="BC69" s="38"/>
+      <c r="BD69" s="38"/>
+      <c r="BE69" s="38"/>
+      <c r="BF69" s="38"/>
       <c r="BG69" s="16"/>
       <c r="BH69" s="16"/>
       <c r="BI69" s="16"/>
@@ -6689,20 +6735,20 @@
       <c r="AP70" s="13"/>
       <c r="AQ70" s="13"/>
       <c r="AR70" s="13"/>
-      <c r="AS70" s="37"/>
-      <c r="AT70" s="37"/>
-      <c r="AU70" s="37"/>
-      <c r="AV70" s="37"/>
-      <c r="AW70" s="37"/>
-      <c r="AX70" s="37"/>
-      <c r="AY70" s="37"/>
-      <c r="AZ70" s="37"/>
-      <c r="BA70" s="37"/>
-      <c r="BB70" s="37"/>
-      <c r="BC70" s="37"/>
-      <c r="BD70" s="37"/>
-      <c r="BE70" s="37"/>
-      <c r="BF70" s="37"/>
+      <c r="AS70" s="38"/>
+      <c r="AT70" s="38"/>
+      <c r="AU70" s="38"/>
+      <c r="AV70" s="38"/>
+      <c r="AW70" s="38"/>
+      <c r="AX70" s="38"/>
+      <c r="AY70" s="38"/>
+      <c r="AZ70" s="38"/>
+      <c r="BA70" s="38"/>
+      <c r="BB70" s="38"/>
+      <c r="BC70" s="38"/>
+      <c r="BD70" s="38"/>
+      <c r="BE70" s="38"/>
+      <c r="BF70" s="38"/>
       <c r="BG70" s="16"/>
       <c r="BH70" s="16"/>
       <c r="BI70" s="16"/>
@@ -6772,20 +6818,20 @@
       <c r="AP71" s="13"/>
       <c r="AQ71" s="13"/>
       <c r="AR71" s="13"/>
-      <c r="AS71" s="37"/>
-      <c r="AT71" s="37"/>
-      <c r="AU71" s="37"/>
-      <c r="AV71" s="37"/>
-      <c r="AW71" s="37"/>
-      <c r="AX71" s="37"/>
-      <c r="AY71" s="37"/>
-      <c r="AZ71" s="37"/>
-      <c r="BA71" s="37"/>
-      <c r="BB71" s="37"/>
-      <c r="BC71" s="37"/>
-      <c r="BD71" s="37"/>
-      <c r="BE71" s="37"/>
-      <c r="BF71" s="37"/>
+      <c r="AS71" s="38"/>
+      <c r="AT71" s="38"/>
+      <c r="AU71" s="38"/>
+      <c r="AV71" s="38"/>
+      <c r="AW71" s="38"/>
+      <c r="AX71" s="38"/>
+      <c r="AY71" s="38"/>
+      <c r="AZ71" s="38"/>
+      <c r="BA71" s="38"/>
+      <c r="BB71" s="38"/>
+      <c r="BC71" s="38"/>
+      <c r="BD71" s="38"/>
+      <c r="BE71" s="38"/>
+      <c r="BF71" s="38"/>
       <c r="BG71" s="16"/>
       <c r="BH71" s="16"/>
       <c r="BI71" s="16"/>
@@ -6855,20 +6901,20 @@
       <c r="AP72" s="13"/>
       <c r="AQ72" s="13"/>
       <c r="AR72" s="13"/>
-      <c r="AS72" s="37"/>
-      <c r="AT72" s="37"/>
-      <c r="AU72" s="37"/>
-      <c r="AV72" s="37"/>
-      <c r="AW72" s="37"/>
-      <c r="AX72" s="37"/>
-      <c r="AY72" s="37"/>
-      <c r="AZ72" s="37"/>
-      <c r="BA72" s="37"/>
-      <c r="BB72" s="37"/>
-      <c r="BC72" s="37"/>
-      <c r="BD72" s="37"/>
-      <c r="BE72" s="37"/>
-      <c r="BF72" s="37"/>
+      <c r="AS72" s="38"/>
+      <c r="AT72" s="38"/>
+      <c r="AU72" s="38"/>
+      <c r="AV72" s="38"/>
+      <c r="AW72" s="38"/>
+      <c r="AX72" s="38"/>
+      <c r="AY72" s="38"/>
+      <c r="AZ72" s="38"/>
+      <c r="BA72" s="38"/>
+      <c r="BB72" s="38"/>
+      <c r="BC72" s="38"/>
+      <c r="BD72" s="38"/>
+      <c r="BE72" s="38"/>
+      <c r="BF72" s="38"/>
       <c r="BG72" s="16"/>
       <c r="BH72" s="16"/>
       <c r="BI72" s="16"/>
@@ -7422,7 +7468,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>10</v>
@@ -7430,17 +7476,17 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7450,7 +7496,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
22.12.18 báo cáo ngày
</commit_message>
<xml_diff>
--- a/DailyReport/DailyReport_DuongLT.xlsx
+++ b/DailyReport/DailyReport_DuongLT.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="84">
   <si>
     <t>No.</t>
   </si>
@@ -251,6 +251,27 @@
   </si>
   <si>
     <t>Hiển thị lại thông báo khi user từ chối chat và khách hàng cố gắng nhắn tin đến</t>
+  </si>
+  <si>
+    <t>Chức năng quản lý PhoneExtent: Chức năng hiển thị danh sash PhoneExtent</t>
+  </si>
+  <si>
+    <t>Chatbox</t>
+  </si>
+  <si>
+    <t>Chức năng quản lý PhoneExtent: Chức năng Sửa PhoneExtent</t>
+  </si>
+  <si>
+    <t>Chức năng quản lý PhoneExtent: Chức năng Sửa PhoneExtent &lt;Tiếp&gt;</t>
+  </si>
+  <si>
+    <t>Chức năng quản lý PhoneExtent: chức năng xóa PhoneExtent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chức năng quản lý PhoneExtent: Chức năng thêm mới PhoneExtent </t>
+  </si>
+  <si>
+    <t>Tạo Bảng User_ExtPhone_Mapping trong database Chatbox</t>
   </si>
 </sst>
 </file>
@@ -518,7 +539,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -591,6 +612,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1078,9 +1102,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CA128"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D97" sqref="D97:AE97"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="BG101" sqref="BG101:CA101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9405,7 +9429,9 @@
       </c>
       <c r="B95" s="11"/>
       <c r="C95" s="5"/>
-      <c r="D95" s="12"/>
+      <c r="D95" s="12" t="s">
+        <v>77</v>
+      </c>
       <c r="E95" s="12"/>
       <c r="F95" s="12"/>
       <c r="G95" s="12"/>
@@ -9433,7 +9459,9 @@
       <c r="AC95" s="12"/>
       <c r="AD95" s="12"/>
       <c r="AE95" s="12"/>
-      <c r="AF95" s="13"/>
+      <c r="AF95" s="13">
+        <v>43455</v>
+      </c>
       <c r="AG95" s="13"/>
       <c r="AH95" s="13"/>
       <c r="AI95" s="13"/>
@@ -9443,10 +9471,14 @@
       <c r="AM95" s="12"/>
       <c r="AN95" s="12"/>
       <c r="AO95" s="12"/>
-      <c r="AP95" s="14"/>
+      <c r="AP95" s="14">
+        <v>1</v>
+      </c>
       <c r="AQ95" s="14"/>
       <c r="AR95" s="14"/>
-      <c r="AS95" s="15"/>
+      <c r="AS95" s="15" t="s">
+        <v>78</v>
+      </c>
       <c r="AT95" s="15"/>
       <c r="AU95" s="15"/>
       <c r="AV95" s="15"/>
@@ -9488,7 +9520,9 @@
       </c>
       <c r="B96" s="11"/>
       <c r="C96" s="5"/>
-      <c r="D96" s="12"/>
+      <c r="D96" s="12" t="s">
+        <v>79</v>
+      </c>
       <c r="E96" s="12"/>
       <c r="F96" s="12"/>
       <c r="G96" s="12"/>
@@ -9516,7 +9550,9 @@
       <c r="AC96" s="12"/>
       <c r="AD96" s="12"/>
       <c r="AE96" s="12"/>
-      <c r="AF96" s="13"/>
+      <c r="AF96" s="13">
+        <v>43455</v>
+      </c>
       <c r="AG96" s="13"/>
       <c r="AH96" s="13"/>
       <c r="AI96" s="13"/>
@@ -9526,10 +9562,14 @@
       <c r="AM96" s="12"/>
       <c r="AN96" s="12"/>
       <c r="AO96" s="12"/>
-      <c r="AP96" s="14"/>
+      <c r="AP96" s="14">
+        <v>0.5</v>
+      </c>
       <c r="AQ96" s="14"/>
       <c r="AR96" s="14"/>
-      <c r="AS96" s="15"/>
+      <c r="AS96" s="15" t="s">
+        <v>78</v>
+      </c>
       <c r="AT96" s="15"/>
       <c r="AU96" s="15"/>
       <c r="AV96" s="15"/>
@@ -9654,7 +9694,9 @@
       </c>
       <c r="B98" s="11"/>
       <c r="C98" s="5"/>
-      <c r="D98" s="12"/>
+      <c r="D98" s="12" t="s">
+        <v>80</v>
+      </c>
       <c r="E98" s="12"/>
       <c r="F98" s="12"/>
       <c r="G98" s="12"/>
@@ -9682,7 +9724,9 @@
       <c r="AC98" s="12"/>
       <c r="AD98" s="12"/>
       <c r="AE98" s="12"/>
-      <c r="AF98" s="13"/>
+      <c r="AF98" s="13">
+        <v>43456</v>
+      </c>
       <c r="AG98" s="13"/>
       <c r="AH98" s="13"/>
       <c r="AI98" s="13"/>
@@ -9692,10 +9736,14 @@
       <c r="AM98" s="12"/>
       <c r="AN98" s="12"/>
       <c r="AO98" s="12"/>
-      <c r="AP98" s="14"/>
+      <c r="AP98" s="14">
+        <v>1</v>
+      </c>
       <c r="AQ98" s="14"/>
       <c r="AR98" s="14"/>
-      <c r="AS98" s="15"/>
+      <c r="AS98" s="15" t="s">
+        <v>78</v>
+      </c>
       <c r="AT98" s="15"/>
       <c r="AU98" s="15"/>
       <c r="AV98" s="15"/>
@@ -9737,7 +9785,9 @@
       </c>
       <c r="B99" s="11"/>
       <c r="C99" s="5"/>
-      <c r="D99" s="12"/>
+      <c r="D99" s="44" t="s">
+        <v>82</v>
+      </c>
       <c r="E99" s="12"/>
       <c r="F99" s="12"/>
       <c r="G99" s="12"/>
@@ -9765,7 +9815,9 @@
       <c r="AC99" s="12"/>
       <c r="AD99" s="12"/>
       <c r="AE99" s="12"/>
-      <c r="AF99" s="13"/>
+      <c r="AF99" s="13">
+        <v>43456</v>
+      </c>
       <c r="AG99" s="13"/>
       <c r="AH99" s="13"/>
       <c r="AI99" s="13"/>
@@ -9775,10 +9827,14 @@
       <c r="AM99" s="12"/>
       <c r="AN99" s="12"/>
       <c r="AO99" s="12"/>
-      <c r="AP99" s="14"/>
+      <c r="AP99" s="14">
+        <v>1</v>
+      </c>
       <c r="AQ99" s="14"/>
       <c r="AR99" s="14"/>
-      <c r="AS99" s="15"/>
+      <c r="AS99" s="15" t="s">
+        <v>78</v>
+      </c>
       <c r="AT99" s="15"/>
       <c r="AU99" s="15"/>
       <c r="AV99" s="15"/>
@@ -9820,7 +9876,9 @@
       </c>
       <c r="B100" s="11"/>
       <c r="C100" s="5"/>
-      <c r="D100" s="12"/>
+      <c r="D100" s="12" t="s">
+        <v>81</v>
+      </c>
       <c r="E100" s="12"/>
       <c r="F100" s="12"/>
       <c r="G100" s="12"/>
@@ -9848,7 +9906,9 @@
       <c r="AC100" s="12"/>
       <c r="AD100" s="12"/>
       <c r="AE100" s="12"/>
-      <c r="AF100" s="13"/>
+      <c r="AF100" s="13">
+        <v>43456</v>
+      </c>
       <c r="AG100" s="13"/>
       <c r="AH100" s="13"/>
       <c r="AI100" s="13"/>
@@ -9858,10 +9918,14 @@
       <c r="AM100" s="12"/>
       <c r="AN100" s="12"/>
       <c r="AO100" s="12"/>
-      <c r="AP100" s="14"/>
+      <c r="AP100" s="14">
+        <v>1</v>
+      </c>
       <c r="AQ100" s="14"/>
       <c r="AR100" s="14"/>
-      <c r="AS100" s="15"/>
+      <c r="AS100" s="15" t="s">
+        <v>78</v>
+      </c>
       <c r="AT100" s="15"/>
       <c r="AU100" s="15"/>
       <c r="AV100" s="15"/>
@@ -9903,7 +9967,9 @@
       </c>
       <c r="B101" s="11"/>
       <c r="C101" s="5"/>
-      <c r="D101" s="12"/>
+      <c r="D101" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="E101" s="12"/>
       <c r="F101" s="12"/>
       <c r="G101" s="12"/>
@@ -9931,7 +9997,9 @@
       <c r="AC101" s="12"/>
       <c r="AD101" s="12"/>
       <c r="AE101" s="12"/>
-      <c r="AF101" s="13"/>
+      <c r="AF101" s="13">
+        <v>43456</v>
+      </c>
       <c r="AG101" s="13"/>
       <c r="AH101" s="13"/>
       <c r="AI101" s="13"/>
@@ -9941,10 +10009,14 @@
       <c r="AM101" s="12"/>
       <c r="AN101" s="12"/>
       <c r="AO101" s="12"/>
-      <c r="AP101" s="14"/>
+      <c r="AP101" s="14">
+        <v>1</v>
+      </c>
       <c r="AQ101" s="14"/>
       <c r="AR101" s="14"/>
-      <c r="AS101" s="15"/>
+      <c r="AS101" s="15" t="s">
+        <v>78</v>
+      </c>
       <c r="AT101" s="15"/>
       <c r="AU101" s="15"/>
       <c r="AV101" s="15"/>
@@ -13082,6 +13154,8 @@
     <mergeCell ref="AP88:AR88"/>
     <mergeCell ref="AS88:BF88"/>
     <mergeCell ref="BG88:CA88"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="A90:B90"/>
     <mergeCell ref="AS93:BF93"/>
     <mergeCell ref="BG93:CA93"/>
     <mergeCell ref="A68:B68"/>
@@ -13106,8 +13180,6 @@
     <mergeCell ref="AP89:AR89"/>
     <mergeCell ref="AS89:BF89"/>
     <mergeCell ref="BG89:CA89"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="A90:B90"/>
     <mergeCell ref="A91:B91"/>
     <mergeCell ref="A92:B92"/>
     <mergeCell ref="A93:B93"/>

</xml_diff>

<commit_message>
29.01.19 - báo cáo
</commit_message>
<xml_diff>
--- a/DailyReport/DailyReport_DuongLT.xlsx
+++ b/DailyReport/DailyReport_DuongLT.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="131">
   <si>
     <t>No.</t>
   </si>
@@ -398,19 +398,22 @@
     <t>Xử lý quyển chỉ có admin mới thêm được staff cho mod</t>
   </si>
   <si>
-    <t>Thêm trang quản lý chat của staff - Giao diện</t>
-  </si>
-  <si>
-    <t>Thêm trang quản lý chat của staff - Chức năng</t>
-  </si>
-  <si>
     <t>Tạo chứ năng phân thêm staff quản trị live chat &lt;Tiếp&gt;</t>
   </si>
   <si>
-    <t>Thêm trang quản lý chat của staff - Giao diện &lt;Tiếp&gt;</t>
+    <t>Thêm trang quản lý chat của staff - Code Giao diện</t>
   </si>
   <si>
-    <t>Thêm trang quản lý chat của staff - Chức năng &lt;Tiếp&gt;</t>
+    <t>Thêm trang quản lý chat của staff - Code Chức năng</t>
+  </si>
+  <si>
+    <t>Thêm trang quản lý chat của staff - Code Giao diện &lt;Tiếp&gt;</t>
+  </si>
+  <si>
+    <t>Thêm trang quản lý chat của staff - Code Chức năng &lt;Tiếp&gt;</t>
+  </si>
+  <si>
+    <t>Hiển thị cuộc chat mới của staff với khách hàng tại trang quản lý chat của mod</t>
   </si>
 </sst>
 </file>
@@ -1287,8 +1290,8 @@
   <dimension ref="A1:F137"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D56" sqref="D56"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1929,7 +1932,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="17" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C47" s="14">
         <v>43488</v>
@@ -1963,7 +1966,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="17" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C49" s="14">
         <v>43488</v>
@@ -1980,7 +1983,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="17" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C50" s="14">
         <v>43488</v>
@@ -2062,6 +2065,18 @@
       <c r="A57" s="15">
         <v>56</v>
       </c>
+      <c r="B57" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="C57" s="14">
+        <v>43493</v>
+      </c>
+      <c r="D57" s="12">
+        <v>0.7</v>
+      </c>
+      <c r="E57" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="15">
@@ -2072,10 +2087,34 @@
       <c r="A59" s="15">
         <v>58</v>
       </c>
+      <c r="B59" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="C59" s="14">
+        <v>43494</v>
+      </c>
+      <c r="D59" s="12">
+        <v>0.99</v>
+      </c>
+      <c r="E59" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="15">
         <v>59</v>
+      </c>
+      <c r="B60" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="C60" s="14">
+        <v>43494</v>
+      </c>
+      <c r="D60" s="12">
+        <v>0.8</v>
+      </c>
+      <c r="E60" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>